<commit_message>
start if rerun timer
</commit_message>
<xml_diff>
--- a/bond_composite.xlsx
+++ b/bond_composite.xlsx
@@ -512,22 +512,22 @@
         <v>47098</v>
       </c>
       <c r="F2" t="n">
-        <v>6.414588354840975</v>
+        <v>6.403577508329116</v>
       </c>
       <c r="G2" t="n">
-        <v>88.54000000000001</v>
+        <v>88.56999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03186212324679216</v>
+        <v>0.03183715456471803</v>
       </c>
       <c r="I2" t="n">
         <v>0.0134</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01846212324679216</v>
+        <v>0.01843715456471803</v>
       </c>
       <c r="K2" t="n">
-        <v>0.03586212324679216</v>
+        <v>0.03663715456471803</v>
       </c>
     </row>
     <row r="3">
@@ -553,22 +553,22 @@
         <v>46736</v>
       </c>
       <c r="F3" t="n">
-        <v>5.422807431545408</v>
+        <v>5.411796627969051</v>
       </c>
       <c r="G3" t="n">
-        <v>95.69</v>
+        <v>95.72</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03558970141998996</v>
+        <v>0.03553937432865162</v>
       </c>
       <c r="I3" t="n">
         <v>0.0123</v>
       </c>
       <c r="J3" t="n">
-        <v>0.02328970141998996</v>
+        <v>0.02323937432865162</v>
       </c>
       <c r="K3" t="n">
-        <v>0.04068970141998996</v>
+        <v>0.04143937432865162</v>
       </c>
     </row>
     <row r="4">
@@ -594,22 +594,22 @@
         <v>48929</v>
       </c>
       <c r="F4" t="n">
-        <v>11.43102651480184</v>
+        <v>11.42001574762284</v>
       </c>
       <c r="G4" t="n">
-        <v>76.72</v>
+        <v>76.84</v>
       </c>
       <c r="H4" t="n">
-        <v>0.03160052427274196</v>
+        <v>0.03147061866053491</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0186</v>
+        <v>0.0191</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01300052427274196</v>
+        <v>0.01237061866053491</v>
       </c>
       <c r="K4" t="n">
-        <v>0.03040052427274196</v>
+        <v>0.03057061866053491</v>
       </c>
     </row>
     <row r="5">
@@ -635,22 +635,22 @@
         <v>47059</v>
       </c>
       <c r="F5" t="n">
-        <v>6.307738759747273</v>
+        <v>6.296728015749271</v>
       </c>
       <c r="G5" t="n">
-        <v>83.84</v>
+        <v>83.78</v>
       </c>
       <c r="H5" t="n">
-        <v>0.02833752748070939</v>
+        <v>0.02850470550880613</v>
       </c>
       <c r="I5" t="n">
         <v>0.0134</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01493752748070939</v>
+        <v>0.01510470550880613</v>
       </c>
       <c r="K5" t="n">
-        <v>0.03233752748070939</v>
+        <v>0.03330470550880613</v>
       </c>
     </row>
     <row r="6">
@@ -676,22 +676,22 @@
         <v>48222</v>
       </c>
       <c r="F6" t="n">
-        <v>9.494040042707921</v>
+        <v>9.483029329420187</v>
       </c>
       <c r="G6" t="n">
-        <v>78.97</v>
+        <v>78.89</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03151177746493539</v>
+        <v>0.03165738164471943</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0166</v>
+        <v>0.0169</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01491177746493539</v>
+        <v>0.01475738164471943</v>
       </c>
       <c r="K6" t="n">
-        <v>0.03231177746493538</v>
+        <v>0.03295738164471943</v>
       </c>
     </row>
     <row r="7">
@@ -707,22 +707,22 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>7.814040220728685</v>
+        <v>7.803029445818093</v>
       </c>
       <c r="G7" t="n">
-        <v>84.75200000000002</v>
+        <v>84.75999999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>0.03178033077703377</v>
+        <v>0.03180184694148602</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01486</v>
+        <v>0.01502</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01692033077703377</v>
+        <v>0.01678184694148602</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03432033077703377</v>
+        <v>0.03498184694148603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>